<commit_message>
race ethniciy data acc finished
</commit_message>
<xml_diff>
--- a/data/race-ethnicity.xlsx
+++ b/data/race-ethnicity.xlsx
@@ -33,9 +33,6 @@
     <t>Black/African American</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>% Hispanic/Latino</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>Asian American</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -461,25 +461,25 @@
         <v>2</v>
       </c>
       <c r="E2">
+        <v>0.0235</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.0588</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
         <v>85</v>
-      </c>
-      <c r="F2">
-        <v>0.0235</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.0588</v>
-      </c>
-      <c r="K2">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -496,25 +496,25 @@
         <v>2</v>
       </c>
       <c r="E3">
+        <v>0.0253</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.0506</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
         <v>79</v>
-      </c>
-      <c r="F3">
-        <v>0.0253</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0.0506</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -531,25 +531,25 @@
         <v>3</v>
       </c>
       <c r="E4">
+        <v>0.0161</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.0645</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
         <v>62</v>
-      </c>
-      <c r="F4">
-        <v>0.0161</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0.0645</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -566,25 +566,25 @@
         <v>3</v>
       </c>
       <c r="E5">
+        <v>0.0172</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.0862</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
         <v>58</v>
-      </c>
-      <c r="F5">
-        <v>0.0172</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0.0862</v>
-      </c>
-      <c r="K5">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -601,25 +601,25 @@
         <v>3</v>
       </c>
       <c r="E6">
+        <v>0.0182</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.0727</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
         <v>55</v>
-      </c>
-      <c r="F6">
-        <v>0.0182</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0.0727</v>
-      </c>
-      <c r="K6">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -636,25 +636,25 @@
         <v>3</v>
       </c>
       <c r="E7">
+        <v>0.0185</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.0185</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.0556</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
         <v>54</v>
-      </c>
-      <c r="F7">
-        <v>0.0185</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0.0185</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0.0556</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -671,25 +671,25 @@
         <v>2</v>
       </c>
       <c r="E8">
+        <v>0.0196</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0.0196</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.0588</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
         <v>51</v>
-      </c>
-      <c r="F8">
-        <v>0.0196</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0.0196</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0.0588</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -706,25 +706,25 @@
         <v>1</v>
       </c>
       <c r="E9">
+        <v>0.0227</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.0227</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0.0682</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
         <v>44</v>
-      </c>
-      <c r="F9">
-        <v>0.0227</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>0.0227</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0.0682</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -741,25 +741,25 @@
         <v>1</v>
       </c>
       <c r="E10">
+        <v>0.0204</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.0204</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0.102</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
         <v>49</v>
-      </c>
-      <c r="F10">
-        <v>0.0204</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0.0204</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0.102</v>
-      </c>
-      <c r="K10">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -776,25 +776,25 @@
         <v>1</v>
       </c>
       <c r="E11">
+        <v>0.0189</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.0377</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>0.09429999999999999</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
         <v>53</v>
-      </c>
-      <c r="F11">
-        <v>0.0189</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0.0377</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-      <c r="J11">
-        <v>0.09429999999999999</v>
-      </c>
-      <c r="K11">
-        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -811,25 +811,25 @@
         <v>1</v>
       </c>
       <c r="E12">
+        <v>0.0175</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0.0351</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>0.1053</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12">
         <v>57</v>
-      </c>
-      <c r="F12">
-        <v>0.0175</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0.0351</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <v>0.1053</v>
-      </c>
-      <c r="K12">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -891,25 +891,25 @@
         <v>1</v>
       </c>
       <c r="E2">
+        <v>0.0738</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>0.008200000000000001</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0.1148</v>
+      </c>
+      <c r="J2">
+        <v>14</v>
+      </c>
+      <c r="K2">
         <v>122</v>
-      </c>
-      <c r="F2">
-        <v>0.0738</v>
-      </c>
-      <c r="G2">
-        <v>9</v>
-      </c>
-      <c r="H2">
-        <v>0.008200000000000001</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0.1148</v>
-      </c>
-      <c r="K2">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -926,25 +926,25 @@
         <v>1</v>
       </c>
       <c r="E3">
+        <v>0.056</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>0.008</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.12</v>
+      </c>
+      <c r="J3">
+        <v>15</v>
+      </c>
+      <c r="K3">
         <v>125</v>
-      </c>
-      <c r="F3">
-        <v>0.056</v>
-      </c>
-      <c r="G3">
-        <v>7</v>
-      </c>
-      <c r="H3">
-        <v>0.008</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0.12</v>
-      </c>
-      <c r="K3">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -961,25 +961,25 @@
         <v>1</v>
       </c>
       <c r="E4">
+        <v>0.07140000000000001</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>0.0089</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0.1339</v>
+      </c>
+      <c r="J4">
+        <v>15</v>
+      </c>
+      <c r="K4">
         <v>112</v>
-      </c>
-      <c r="F4">
-        <v>0.07140000000000001</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-      <c r="H4">
-        <v>0.0089</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0.1339</v>
-      </c>
-      <c r="K4">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -996,25 +996,25 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.0588</v>
       </c>
       <c r="F5">
-        <v>0.0588</v>
+        <v>7</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>0.008399999999999999</v>
       </c>
       <c r="H5">
-        <v>0.008399999999999999</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0.1261</v>
       </c>
       <c r="J5">
-        <v>0.1261</v>
+        <v>15</v>
       </c>
       <c r="K5">
-        <v>15</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1031,25 +1031,25 @@
         <v>1</v>
       </c>
       <c r="E6">
+        <v>0.0703</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>0.0078</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0.1406</v>
+      </c>
+      <c r="J6">
+        <v>18</v>
+      </c>
+      <c r="K6">
         <v>128</v>
-      </c>
-      <c r="F6">
-        <v>0.0703</v>
-      </c>
-      <c r="G6">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>0.0078</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0.1406</v>
-      </c>
-      <c r="K6">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1066,25 +1066,25 @@
         <v>3</v>
       </c>
       <c r="E7">
+        <v>0.0511</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>0.0073</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.1314</v>
+      </c>
+      <c r="J7">
+        <v>18</v>
+      </c>
+      <c r="K7">
         <v>137</v>
-      </c>
-      <c r="F7">
-        <v>0.0511</v>
-      </c>
-      <c r="G7">
-        <v>7</v>
-      </c>
-      <c r="H7">
-        <v>0.0073</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0.1314</v>
-      </c>
-      <c r="K7">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1101,25 +1101,25 @@
         <v>2</v>
       </c>
       <c r="E8">
+        <v>0.0408</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>0.0068</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.1429</v>
+      </c>
+      <c r="J8">
+        <v>21</v>
+      </c>
+      <c r="K8">
         <v>147</v>
-      </c>
-      <c r="F8">
-        <v>0.0408</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-      <c r="H8">
-        <v>0.0068</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0.1429</v>
-      </c>
-      <c r="K8">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1136,25 +1136,25 @@
         <v>4</v>
       </c>
       <c r="E9">
+        <v>0.0494</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>0.0123</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>0.1358</v>
+      </c>
+      <c r="J9">
+        <v>22</v>
+      </c>
+      <c r="K9">
         <v>162</v>
-      </c>
-      <c r="F9">
-        <v>0.0494</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
-      </c>
-      <c r="H9">
-        <v>0.0123</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>0.1358</v>
-      </c>
-      <c r="K9">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1171,25 +1171,25 @@
         <v>3</v>
       </c>
       <c r="E10">
+        <v>0.0859</v>
+      </c>
+      <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>0.0061</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0.1411</v>
+      </c>
+      <c r="J10">
+        <v>23</v>
+      </c>
+      <c r="K10">
         <v>163</v>
-      </c>
-      <c r="F10">
-        <v>0.0859</v>
-      </c>
-      <c r="G10">
-        <v>14</v>
-      </c>
-      <c r="H10">
-        <v>0.0061</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0.1411</v>
-      </c>
-      <c r="K10">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1206,25 +1206,25 @@
         <v>3</v>
       </c>
       <c r="E11">
+        <v>0.0756</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>0.0116</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>0.1337</v>
+      </c>
+      <c r="J11">
+        <v>23</v>
+      </c>
+      <c r="K11">
         <v>172</v>
-      </c>
-      <c r="F11">
-        <v>0.0756</v>
-      </c>
-      <c r="G11">
-        <v>13</v>
-      </c>
-      <c r="H11">
-        <v>0.0116</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-      <c r="J11">
-        <v>0.1337</v>
-      </c>
-      <c r="K11">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1241,25 +1241,25 @@
         <v>2</v>
       </c>
       <c r="E12">
+        <v>0.0769</v>
+      </c>
+      <c r="F12">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>0.0118</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>0.1538</v>
+      </c>
+      <c r="J12">
+        <v>26</v>
+      </c>
+      <c r="K12">
         <v>169</v>
-      </c>
-      <c r="F12">
-        <v>0.0769</v>
-      </c>
-      <c r="G12">
-        <v>13</v>
-      </c>
-      <c r="H12">
-        <v>0.0118</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <v>0.1538</v>
-      </c>
-      <c r="K12">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1292,7 +1292,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -1315,19 +1315,19 @@
         <v>7</v>
       </c>
       <c r="E2">
+        <v>0.0246</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>0.082</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
         <v>122</v>
-      </c>
-      <c r="F2">
-        <v>0.0246</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>0.082</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1344,19 +1344,19 @@
         <v>8</v>
       </c>
       <c r="E3">
+        <v>0.0376</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>0.0752</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
         <v>133</v>
-      </c>
-      <c r="F3">
-        <v>0.0376</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>0.0752</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1373,19 +1373,19 @@
         <v>9</v>
       </c>
       <c r="E4">
+        <v>0.0426</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>0.078</v>
+      </c>
+      <c r="H4">
+        <v>11</v>
+      </c>
+      <c r="I4">
         <v>141</v>
-      </c>
-      <c r="F4">
-        <v>0.0426</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>0.078</v>
-      </c>
-      <c r="I4">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1402,19 +1402,19 @@
         <v>9</v>
       </c>
       <c r="E5">
+        <v>0.037</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>0.0815</v>
+      </c>
+      <c r="H5">
+        <v>11</v>
+      </c>
+      <c r="I5">
         <v>135</v>
-      </c>
-      <c r="F5">
-        <v>0.037</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>0.0815</v>
-      </c>
-      <c r="I5">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1431,19 +1431,19 @@
         <v>9</v>
       </c>
       <c r="E6">
+        <v>0.0357</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>0.0786</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+      <c r="I6">
         <v>140</v>
-      </c>
-      <c r="F6">
-        <v>0.0357</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>0.0786</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1460,19 +1460,19 @@
         <v>9</v>
       </c>
       <c r="E7">
+        <v>0.0352</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>0.0775</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
         <v>142</v>
-      </c>
-      <c r="F7">
-        <v>0.0352</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>0.0775</v>
-      </c>
-      <c r="I7">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1489,19 +1489,19 @@
         <v>10</v>
       </c>
       <c r="E8">
+        <v>0.034</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>0.08160000000000001</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
         <v>147</v>
-      </c>
-      <c r="F8">
-        <v>0.034</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>0.08160000000000001</v>
-      </c>
-      <c r="I8">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1518,19 +1518,19 @@
         <v>11</v>
       </c>
       <c r="E9">
+        <v>0.0331</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>0.0795</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="I9">
         <v>151</v>
-      </c>
-      <c r="F9">
-        <v>0.0331</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>0.0795</v>
-      </c>
-      <c r="I9">
-        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1547,19 +1547,19 @@
         <v>11</v>
       </c>
       <c r="E10">
+        <v>0.0329</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>0.08550000000000001</v>
+      </c>
+      <c r="H10">
+        <v>13</v>
+      </c>
+      <c r="I10">
         <v>152</v>
-      </c>
-      <c r="F10">
-        <v>0.0329</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>0.08550000000000001</v>
-      </c>
-      <c r="I10">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1576,19 +1576,19 @@
         <v>12</v>
       </c>
       <c r="E11">
+        <v>0.0329</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>0.08550000000000001</v>
+      </c>
+      <c r="H11">
+        <v>13</v>
+      </c>
+      <c r="I11">
         <v>152</v>
-      </c>
-      <c r="F11">
-        <v>0.0329</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>0.08550000000000001</v>
-      </c>
-      <c r="I11">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1605,19 +1605,19 @@
         <v>12</v>
       </c>
       <c r="E12">
+        <v>0.0327</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="H12">
+        <v>13</v>
+      </c>
+      <c r="I12">
         <v>153</v>
-      </c>
-      <c r="F12">
-        <v>0.0327</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <v>0.08500000000000001</v>
-      </c>
-      <c r="I12">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1679,25 +1679,25 @@
         <v>1</v>
       </c>
       <c r="E2">
+        <v>0.0167</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.0333</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
         <v>60</v>
-      </c>
-      <c r="F2">
-        <v>0.0167</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.0333</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1714,25 +1714,25 @@
         <v>1</v>
       </c>
       <c r="E3">
+        <v>0.0313</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.0469</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
         <v>64</v>
-      </c>
-      <c r="F3">
-        <v>0.0313</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0.0469</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1749,25 +1749,25 @@
         <v>1</v>
       </c>
       <c r="E4">
+        <v>0.0313</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.0625</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
         <v>64</v>
-      </c>
-      <c r="F4">
-        <v>0.0313</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0.0625</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1784,25 +1784,25 @@
         <v>1</v>
       </c>
       <c r="E5">
+        <v>0.0448</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>0.0149</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0.0746</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
         <v>67</v>
-      </c>
-      <c r="F5">
-        <v>0.0448</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>0.0149</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0.0746</v>
-      </c>
-      <c r="K5">
-        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1819,25 +1819,25 @@
         <v>1</v>
       </c>
       <c r="E6">
+        <v>0.0563</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>0.0141</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0.1268</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6">
         <v>71</v>
-      </c>
-      <c r="F6">
-        <v>0.0563</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>0.0141</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0.1268</v>
-      </c>
-      <c r="K6">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1854,25 +1854,25 @@
         <v>1</v>
       </c>
       <c r="E7">
+        <v>0.029</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>0.029</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>0.1014</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+      <c r="K7">
         <v>69</v>
-      </c>
-      <c r="F7">
-        <v>0.029</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <v>0.029</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <v>0.1014</v>
-      </c>
-      <c r="K7">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1889,25 +1889,25 @@
         <v>1</v>
       </c>
       <c r="E8">
+        <v>0.0282</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0.0282</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>0.1408</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
         <v>71</v>
-      </c>
-      <c r="F8">
-        <v>0.0282</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>0.0282</v>
-      </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>0.1408</v>
-      </c>
-      <c r="K8">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1924,25 +1924,25 @@
         <v>1</v>
       </c>
       <c r="E9">
+        <v>0.0323</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>0.0323</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>0.1129</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
         <v>62</v>
-      </c>
-      <c r="F9">
-        <v>0.0323</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9">
-        <v>0.0323</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>0.1129</v>
-      </c>
-      <c r="K9">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1959,25 +1959,25 @@
         <v>1</v>
       </c>
       <c r="E10">
+        <v>0.037</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>0.037</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>0.0556</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
         <v>54</v>
-      </c>
-      <c r="F10">
-        <v>0.037</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>0.037</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>0.0556</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1994,25 +1994,25 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.0392</v>
       </c>
       <c r="F11">
-        <v>0.0392</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>0.0196</v>
       </c>
       <c r="H11">
-        <v>0.0196</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0.0588</v>
       </c>
       <c r="J11">
-        <v>0.0588</v>
+        <v>3</v>
       </c>
       <c r="K11">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2029,25 +2029,25 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="F12">
-        <v>0.04</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="J12">
-        <v>0.08</v>
+        <v>4</v>
       </c>
       <c r="K12">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2109,25 +2109,25 @@
         <v>1</v>
       </c>
       <c r="E2">
+        <v>0.09089999999999999</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.0455</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
         <v>22</v>
-      </c>
-      <c r="F2">
-        <v>0.09089999999999999</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.0455</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2144,25 +2144,25 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.1053</v>
       </c>
       <c r="F3">
-        <v>0.1053</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.0526</v>
       </c>
       <c r="J3">
-        <v>0.0526</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2179,25 +2179,25 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F4">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J4">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2214,25 +2214,25 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.0435</v>
       </c>
       <c r="F5">
-        <v>0.0435</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="J5">
-        <v>0.08699999999999999</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2249,25 +2249,25 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.0313</v>
       </c>
       <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>0.0313</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
       <c r="H6">
-        <v>0.0313</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="J6">
-        <v>0.0625</v>
+        <v>2</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2284,25 +2284,25 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.027</v>
       </c>
       <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>0.027</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
       <c r="H7">
-        <v>0.027</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0.0541</v>
       </c>
       <c r="J7">
-        <v>0.0541</v>
+        <v>2</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2319,25 +2319,25 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.0541</v>
       </c>
       <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>0.0541</v>
       </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
       <c r="J8">
-        <v>0.0541</v>
+        <v>2</v>
       </c>
       <c r="K8">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2354,25 +2354,25 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.0278</v>
       </c>
       <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>0.0278</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
       <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>0.0278</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
       <c r="J9">
-        <v>0.0278</v>
+        <v>1</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2389,25 +2389,25 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.027</v>
       </c>
       <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>0.027</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
       <c r="H10">
-        <v>0.027</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0.0541</v>
       </c>
       <c r="J10">
-        <v>0.0541</v>
+        <v>2</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2424,25 +2424,25 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.0769</v>
       </c>
       <c r="F11">
-        <v>0.0769</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>0.0192</v>
       </c>
       <c r="H11">
-        <v>0.0192</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0.0385</v>
       </c>
       <c r="J11">
-        <v>0.0385</v>
+        <v>2</v>
       </c>
       <c r="K11">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2459,25 +2459,25 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.0417</v>
       </c>
       <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0.0208</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>0.0417</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>0.0208</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
       <c r="J12">
-        <v>0.0417</v>
+        <v>2</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2539,25 +2539,25 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.0221</v>
       </c>
       <c r="F2">
-        <v>0.0221</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.0809</v>
       </c>
       <c r="J2">
-        <v>0.0809</v>
+        <v>11</v>
       </c>
       <c r="K2">
-        <v>11</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2574,25 +2574,25 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.0221</v>
       </c>
       <c r="F3">
-        <v>0.0221</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.0809</v>
       </c>
       <c r="J3">
-        <v>0.0809</v>
+        <v>11</v>
       </c>
       <c r="K3">
-        <v>11</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2609,25 +2609,25 @@
         <v>2</v>
       </c>
       <c r="E4">
+        <v>0.0214</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.0857</v>
+      </c>
+      <c r="J4">
+        <v>12</v>
+      </c>
+      <c r="K4">
         <v>140</v>
-      </c>
-      <c r="F4">
-        <v>0.0214</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0.0857</v>
-      </c>
-      <c r="K4">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2644,25 +2644,25 @@
         <v>2</v>
       </c>
       <c r="E5">
+        <v>0.0214</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.0929</v>
+      </c>
+      <c r="J5">
+        <v>13</v>
+      </c>
+      <c r="K5">
         <v>140</v>
-      </c>
-      <c r="F5">
-        <v>0.0214</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0.0929</v>
-      </c>
-      <c r="K5">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2679,25 +2679,25 @@
         <v>1</v>
       </c>
       <c r="E6">
+        <v>0.021</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.09089999999999999</v>
+      </c>
+      <c r="J6">
+        <v>13</v>
+      </c>
+      <c r="K6">
         <v>143</v>
-      </c>
-      <c r="F6">
-        <v>0.021</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0.09089999999999999</v>
-      </c>
-      <c r="K6">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2714,25 +2714,25 @@
         <v>1</v>
       </c>
       <c r="E7">
+        <v>0.027</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.0946</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+      <c r="K7">
         <v>148</v>
-      </c>
-      <c r="F7">
-        <v>0.027</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0.0946</v>
-      </c>
-      <c r="K7">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2749,25 +2749,25 @@
         <v>1</v>
       </c>
       <c r="E8">
+        <v>0.0258</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0.09030000000000001</v>
+      </c>
+      <c r="J8">
+        <v>14</v>
+      </c>
+      <c r="K8">
         <v>155</v>
-      </c>
-      <c r="F8">
-        <v>0.0258</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0.09030000000000001</v>
-      </c>
-      <c r="K8">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2784,25 +2784,25 @@
         <v>1</v>
       </c>
       <c r="E9">
+        <v>0.0309</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0.0926</v>
+      </c>
+      <c r="J9">
+        <v>15</v>
+      </c>
+      <c r="K9">
         <v>162</v>
-      </c>
-      <c r="F9">
-        <v>0.0309</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0.0926</v>
-      </c>
-      <c r="K9">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2819,25 +2819,25 @@
         <v>1</v>
       </c>
       <c r="E10">
+        <v>0.0311</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.1056</v>
+      </c>
+      <c r="J10">
+        <v>17</v>
+      </c>
+      <c r="K10">
         <v>161</v>
-      </c>
-      <c r="F10">
-        <v>0.0311</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0.1056</v>
-      </c>
-      <c r="K10">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2854,25 +2854,25 @@
         <v>2</v>
       </c>
       <c r="E11">
+        <v>0.0303</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>0.0061</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0.1091</v>
+      </c>
+      <c r="J11">
+        <v>18</v>
+      </c>
+      <c r="K11">
         <v>165</v>
-      </c>
-      <c r="F11">
-        <v>0.0303</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>0.0061</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0.1091</v>
-      </c>
-      <c r="K11">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2889,25 +2889,25 @@
         <v>2</v>
       </c>
       <c r="E12">
+        <v>0.0347</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>0.0116</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>0.104</v>
+      </c>
+      <c r="J12">
+        <v>18</v>
+      </c>
+      <c r="K12">
         <v>173</v>
-      </c>
-      <c r="F12">
-        <v>0.0347</v>
-      </c>
-      <c r="G12">
-        <v>6</v>
-      </c>
-      <c r="H12">
-        <v>0.0116</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <v>0.104</v>
-      </c>
-      <c r="K12">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2940,7 +2940,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>8</v>
@@ -2963,19 +2963,19 @@
         <v>1</v>
       </c>
       <c r="E2">
+        <v>0.0238</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.09520000000000001</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
         <v>42</v>
-      </c>
-      <c r="F2">
-        <v>0.0238</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>0.09520000000000001</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2992,19 +2992,19 @@
         <v>4</v>
       </c>
       <c r="E3">
+        <v>0.0208</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0.1042</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
         <v>48</v>
-      </c>
-      <c r="F3">
-        <v>0.0208</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>0.1042</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3021,19 +3021,19 @@
         <v>5</v>
       </c>
       <c r="E4">
+        <v>0.0217</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
         <v>46</v>
-      </c>
-      <c r="F4">
-        <v>0.0217</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0.08699999999999999</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3050,19 +3050,19 @@
         <v>4</v>
       </c>
       <c r="E5">
+        <v>0.0222</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0.08890000000000001</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
         <v>45</v>
-      </c>
-      <c r="F5">
-        <v>0.0222</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0.08890000000000001</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3079,19 +3079,19 @@
         <v>4</v>
       </c>
       <c r="E6">
+        <v>0.0204</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.08160000000000001</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
         <v>49</v>
-      </c>
-      <c r="F6">
-        <v>0.0204</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0.08160000000000001</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3108,19 +3108,19 @@
         <v>5</v>
       </c>
       <c r="E7">
+        <v>0.0204</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.102</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
         <v>49</v>
-      </c>
-      <c r="F7">
-        <v>0.0204</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0.102</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3137,19 +3137,19 @@
         <v>4</v>
       </c>
       <c r="E8">
+        <v>0.0444</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0.1111</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
         <v>45</v>
-      </c>
-      <c r="F8">
-        <v>0.0444</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>0.1111</v>
-      </c>
-      <c r="I8">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3166,19 +3166,19 @@
         <v>4</v>
       </c>
       <c r="E9">
+        <v>0.025</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.125</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
         <v>40</v>
-      </c>
-      <c r="F9">
-        <v>0.025</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>0.125</v>
-      </c>
-      <c r="I9">
-        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3195,19 +3195,19 @@
         <v>3</v>
       </c>
       <c r="E10">
+        <v>0.0294</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.0882</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
         <v>34</v>
-      </c>
-      <c r="F10">
-        <v>0.0294</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0.0882</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3224,19 +3224,19 @@
         <v>3</v>
       </c>
       <c r="E11">
+        <v>0.027</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.08110000000000001</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
         <v>37</v>
-      </c>
-      <c r="F11">
-        <v>0.027</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0.08110000000000001</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3253,19 +3253,19 @@
         <v>2</v>
       </c>
       <c r="E12">
+        <v>0.0476</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>0.07140000000000001</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
         <v>42</v>
-      </c>
-      <c r="F12">
-        <v>0.0476</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>0.07140000000000001</v>
-      </c>
-      <c r="I12">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3327,25 +3327,25 @@
         <v>2</v>
       </c>
       <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
         <v>20</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0.1</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3362,25 +3362,25 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.0526</v>
       </c>
       <c r="F3">
-        <v>0.0526</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.1053</v>
       </c>
       <c r="J3">
-        <v>0.1053</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3397,25 +3397,25 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.0588</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>0.0588</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
       <c r="J4">
-        <v>0.0588</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -3444,13 +3444,13 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.1429</v>
       </c>
       <c r="J5">
-        <v>0.1429</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -3467,25 +3467,25 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.0455</v>
       </c>
       <c r="F6">
-        <v>0.0455</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.1364</v>
       </c>
       <c r="J6">
-        <v>0.1364</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -3502,25 +3502,25 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F7">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J7">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="K7">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -3537,25 +3537,25 @@
         <v>1</v>
       </c>
       <c r="E8">
+        <v>0.0294</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0.1176</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
         <v>34</v>
-      </c>
-      <c r="F8">
-        <v>0.0294</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0.1176</v>
-      </c>
-      <c r="K8">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3572,25 +3572,25 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.0303</v>
       </c>
       <c r="F9">
-        <v>0.0303</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>0.0606</v>
       </c>
       <c r="J9">
-        <v>0.0606</v>
+        <v>2</v>
       </c>
       <c r="K9">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -3607,25 +3607,25 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.0571</v>
       </c>
       <c r="F10">
-        <v>0.0571</v>
+        <v>2</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.0286</v>
       </c>
       <c r="J10">
-        <v>0.0286</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -3642,25 +3642,25 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.0227</v>
       </c>
       <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
         <v>0.0227</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
       <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>0.0227</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
       <c r="J11">
-        <v>0.0227</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -3677,25 +3677,25 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.0263</v>
       </c>
       <c r="F12">
-        <v>0.0263</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0.0526</v>
       </c>
       <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
         <v>0.0526</v>
       </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
       <c r="J12">
-        <v>0.0526</v>
+        <v>2</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3757,25 +3757,25 @@
         <v>4</v>
       </c>
       <c r="E2">
+        <v>0.0354</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>0.008800000000000001</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0.0885</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
         <v>113</v>
-      </c>
-      <c r="F2">
-        <v>0.0354</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>0.008800000000000001</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0.0885</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3792,25 +3792,25 @@
         <v>5</v>
       </c>
       <c r="E3">
+        <v>0.0427</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>0.008500000000000001</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.094</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3">
         <v>117</v>
-      </c>
-      <c r="F3">
-        <v>0.0427</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>0.008500000000000001</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0.094</v>
-      </c>
-      <c r="K3">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3827,25 +3827,25 @@
         <v>5</v>
       </c>
       <c r="E4">
+        <v>0.0492</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>0.008200000000000001</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0.1148</v>
+      </c>
+      <c r="J4">
+        <v>14</v>
+      </c>
+      <c r="K4">
         <v>122</v>
-      </c>
-      <c r="F4">
-        <v>0.0492</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>0.008200000000000001</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0.1148</v>
-      </c>
-      <c r="K4">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -3862,25 +3862,25 @@
         <v>6</v>
       </c>
       <c r="E5">
+        <v>0.0496</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>0.0083</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0.124</v>
+      </c>
+      <c r="J5">
+        <v>15</v>
+      </c>
+      <c r="K5">
         <v>121</v>
-      </c>
-      <c r="F5">
-        <v>0.0496</v>
-      </c>
-      <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>0.0083</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0.124</v>
-      </c>
-      <c r="K5">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -3897,25 +3897,25 @@
         <v>6</v>
       </c>
       <c r="E6">
+        <v>0.0492</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>0.008200000000000001</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0.123</v>
+      </c>
+      <c r="J6">
+        <v>15</v>
+      </c>
+      <c r="K6">
         <v>122</v>
-      </c>
-      <c r="F6">
-        <v>0.0492</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6">
-        <v>0.008200000000000001</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0.123</v>
-      </c>
-      <c r="K6">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -3932,25 +3932,25 @@
         <v>6</v>
       </c>
       <c r="E7">
+        <v>0.0417</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>0.0083</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.1167</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+      <c r="K7">
         <v>120</v>
-      </c>
-      <c r="F7">
-        <v>0.0417</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>0.0083</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0.1167</v>
-      </c>
-      <c r="K7">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -3967,25 +3967,25 @@
         <v>7</v>
       </c>
       <c r="E8">
+        <v>0.041</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>0.008200000000000001</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.1066</v>
+      </c>
+      <c r="J8">
+        <v>13</v>
+      </c>
+      <c r="K8">
         <v>122</v>
-      </c>
-      <c r="F8">
-        <v>0.041</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>0.008200000000000001</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>0.1066</v>
-      </c>
-      <c r="K8">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -4002,25 +4002,25 @@
         <v>7</v>
       </c>
       <c r="E9">
+        <v>0.0403</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>0.0081</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0.1048</v>
+      </c>
+      <c r="J9">
+        <v>13</v>
+      </c>
+      <c r="K9">
         <v>124</v>
-      </c>
-      <c r="F9">
-        <v>0.0403</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>0.0081</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0.1048</v>
-      </c>
-      <c r="K9">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -4037,25 +4037,25 @@
         <v>7</v>
       </c>
       <c r="E10">
+        <v>0.04</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>0.008</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0.104</v>
+      </c>
+      <c r="J10">
+        <v>13</v>
+      </c>
+      <c r="K10">
         <v>125</v>
-      </c>
-      <c r="F10">
-        <v>0.04</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <v>0.008</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0.104</v>
-      </c>
-      <c r="K10">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -4072,25 +4072,25 @@
         <v>8</v>
       </c>
       <c r="E11">
+        <v>0.0469</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>0.0078</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0.1172</v>
+      </c>
+      <c r="J11">
+        <v>15</v>
+      </c>
+      <c r="K11">
         <v>128</v>
-      </c>
-      <c r="F11">
-        <v>0.0469</v>
-      </c>
-      <c r="G11">
-        <v>6</v>
-      </c>
-      <c r="H11">
-        <v>0.0078</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0.1172</v>
-      </c>
-      <c r="K11">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -4107,25 +4107,25 @@
         <v>8</v>
       </c>
       <c r="E12">
+        <v>0.0458</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>0.0076</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0.1221</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
         <v>131</v>
-      </c>
-      <c r="F12">
-        <v>0.0458</v>
-      </c>
-      <c r="G12">
-        <v>6</v>
-      </c>
-      <c r="H12">
-        <v>0.0076</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>0.1221</v>
-      </c>
-      <c r="K12">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>